<commit_message>
Function to standarize data
</commit_message>
<xml_diff>
--- a/data/clean/cleaned_data.xlsx
+++ b/data/clean/cleaned_data.xlsx
@@ -73,7 +73,7 @@
     <t>Luftanhalten (s)</t>
   </si>
   <si>
-    <t>Häufigkeit Blinken</t>
+    <t>Häufigkeit Blinzeln (/min)</t>
   </si>
   <si>
     <t>Studierende</t>
@@ -595,7 +595,7 @@
         <v>53</v>
       </c>
       <c r="T2">
-        <v>66</v>
+        <v>34.13793103448276</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -657,7 +657,7 @@
         <v>120</v>
       </c>
       <c r="T3">
-        <v>88</v>
+        <v>45.51724137931034</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -719,7 +719,7 @@
         <v>60</v>
       </c>
       <c r="T4">
-        <v>20</v>
+        <v>10.3448275862069</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -834,7 +834,7 @@
         <v>51.5</v>
       </c>
       <c r="T6">
-        <v>17</v>
+        <v>8.793103448275861</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -896,7 +896,7 @@
         <v>72</v>
       </c>
       <c r="T7">
-        <v>30</v>
+        <v>15.51724137931035</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -958,7 +958,7 @@
         <v>80</v>
       </c>
       <c r="T8">
-        <v>32</v>
+        <v>16.55172413793104</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1020,7 +1020,7 @@
         <v>75</v>
       </c>
       <c r="T9">
-        <v>21</v>
+        <v>10.86206896551724</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1111,7 +1111,7 @@
         <v>91</v>
       </c>
       <c r="T11">
-        <v>30</v>
+        <v>15.51724137931035</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1173,7 +1173,7 @@
         <v>73</v>
       </c>
       <c r="T12">
-        <v>16</v>
+        <v>8.275862068965518</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1235,7 +1235,7 @@
         <v>50</v>
       </c>
       <c r="T13">
-        <v>16</v>
+        <v>8.275862068965518</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1350,7 +1350,7 @@
         <v>97</v>
       </c>
       <c r="T15">
-        <v>15</v>
+        <v>7.758620689655173</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1462,7 +1462,7 @@
         <v>71</v>
       </c>
       <c r="T17">
-        <v>51</v>
+        <v>26.37931034482759</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -1642,7 +1642,7 @@
         <v>49</v>
       </c>
       <c r="T20">
-        <v>5</v>
+        <v>2.586206896551724</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -1704,7 +1704,7 @@
         <v>92</v>
       </c>
       <c r="T21">
-        <v>28</v>
+        <v>14.48275862068966</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -1766,7 +1766,7 @@
         <v>41</v>
       </c>
       <c r="T22">
-        <v>18</v>
+        <v>9.310344827586206</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -1934,7 +1934,7 @@
         <v>70</v>
       </c>
       <c r="T25">
-        <v>15</v>
+        <v>7.758620689655173</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -1996,7 +1996,7 @@
         <v>40</v>
       </c>
       <c r="T26">
-        <v>1</v>
+        <v>0.5172413793103449</v>
       </c>
     </row>
     <row r="27" spans="1:20">
@@ -2058,7 +2058,7 @@
         <v>70</v>
       </c>
       <c r="T27">
-        <v>7</v>
+        <v>3.620689655172414</v>
       </c>
     </row>
     <row r="28" spans="1:20">
@@ -2120,7 +2120,7 @@
         <v>40</v>
       </c>
       <c r="T28">
-        <v>41</v>
+        <v>21.20689655172414</v>
       </c>
     </row>
     <row r="29" spans="1:20">
@@ -2241,7 +2241,7 @@
         <v>65</v>
       </c>
       <c r="T30">
-        <v>17</v>
+        <v>8.793103448275861</v>
       </c>
     </row>
     <row r="31" spans="1:20">
@@ -2362,7 +2362,7 @@
         <v>58</v>
       </c>
       <c r="T32">
-        <v>33</v>
+        <v>17.06896551724138</v>
       </c>
     </row>
     <row r="33" spans="1:20">
@@ -2719,7 +2719,7 @@
         <v>52</v>
       </c>
       <c r="T38">
-        <v>16</v>
+        <v>8.275862068965518</v>
       </c>
     </row>
     <row r="39" spans="1:20">
@@ -2896,7 +2896,7 @@
         <v>47</v>
       </c>
       <c r="T41">
-        <v>66</v>
+        <v>34.13793103448276</v>
       </c>
     </row>
     <row r="42" spans="1:20">
@@ -2958,7 +2958,7 @@
         <v>40</v>
       </c>
       <c r="T42">
-        <v>6</v>
+        <v>3.103448275862069</v>
       </c>
     </row>
     <row r="43" spans="1:20">
@@ -3129,7 +3129,7 @@
         <v>58.5</v>
       </c>
       <c r="T45">
-        <v>9</v>
+        <v>4.655172413793103</v>
       </c>
     </row>
     <row r="46" spans="1:20">
@@ -3179,7 +3179,7 @@
         <v>51.45</v>
       </c>
       <c r="T46">
-        <v>22</v>
+        <v>11.37931034482759</v>
       </c>
     </row>
     <row r="47" spans="1:20">
@@ -3229,7 +3229,7 @@
         <v>39</v>
       </c>
       <c r="T47">
-        <v>31</v>
+        <v>16.03448275862069</v>
       </c>
     </row>
     <row r="48" spans="1:20">
@@ -3291,7 +3291,7 @@
         <v>31</v>
       </c>
       <c r="T48">
-        <v>63</v>
+        <v>32.58620689655173</v>
       </c>
     </row>
     <row r="49" spans="1:20">
@@ -3353,7 +3353,7 @@
         <v>44</v>
       </c>
       <c r="T49">
-        <v>46</v>
+        <v>23.79310344827586</v>
       </c>
     </row>
     <row r="50" spans="1:20">
@@ -3639,7 +3639,7 @@
         <v>30</v>
       </c>
       <c r="T54">
-        <v>20</v>
+        <v>10.3448275862069</v>
       </c>
     </row>
     <row r="55" spans="1:20">
@@ -3701,7 +3701,7 @@
         <v>65</v>
       </c>
       <c r="T55">
-        <v>59</v>
+        <v>30.51724137931034</v>
       </c>
     </row>
     <row r="56" spans="1:20">
@@ -3763,7 +3763,7 @@
         <v>54</v>
       </c>
       <c r="T56">
-        <v>16</v>
+        <v>8.275862068965518</v>
       </c>
     </row>
     <row r="57" spans="1:20">
@@ -3881,7 +3881,7 @@
         <v>24.25</v>
       </c>
       <c r="T58">
-        <v>17</v>
+        <v>8.793103448275861</v>
       </c>
     </row>
     <row r="59" spans="1:20">
@@ -3943,7 +3943,7 @@
         <v>38</v>
       </c>
       <c r="T59">
-        <v>33</v>
+        <v>17.06896551724138</v>
       </c>
     </row>
     <row r="60" spans="1:20">
@@ -4064,7 +4064,7 @@
         <v>50</v>
       </c>
       <c r="T61">
-        <v>15</v>
+        <v>7.758620689655173</v>
       </c>
     </row>
     <row r="62" spans="1:20">
@@ -4126,7 +4126,7 @@
         <v>71</v>
       </c>
       <c r="T62">
-        <v>19</v>
+        <v>9.827586206896552</v>
       </c>
     </row>
     <row r="63" spans="1:20">
@@ -4182,7 +4182,7 @@
         <v>35</v>
       </c>
       <c r="T63">
-        <v>1</v>
+        <v>0.5172413793103449</v>
       </c>
     </row>
     <row r="64" spans="1:20">
@@ -4244,7 +4244,7 @@
         <v>85</v>
       </c>
       <c r="T64">
-        <v>8</v>
+        <v>4.137931034482759</v>
       </c>
     </row>
     <row r="65" spans="1:20">
@@ -4306,7 +4306,7 @@
         <v>53</v>
       </c>
       <c r="T65">
-        <v>16</v>
+        <v>8.275862068965518</v>
       </c>
     </row>
     <row r="66" spans="1:20">
@@ -4356,7 +4356,7 @@
         <v>55</v>
       </c>
       <c r="T66">
-        <v>24</v>
+        <v>12.41379310344828</v>
       </c>
     </row>
     <row r="67" spans="1:20">
@@ -4418,7 +4418,7 @@
         <v>90</v>
       </c>
       <c r="T67">
-        <v>9</v>
+        <v>4.655172413793103</v>
       </c>
     </row>
     <row r="68" spans="1:20">
@@ -4480,7 +4480,7 @@
         <v>55</v>
       </c>
       <c r="T68">
-        <v>45</v>
+        <v>23.27586206896552</v>
       </c>
     </row>
     <row r="69" spans="1:20">
@@ -4542,7 +4542,7 @@
         <v>143</v>
       </c>
       <c r="T69">
-        <v>12</v>
+        <v>6.206896551724138</v>
       </c>
     </row>
     <row r="70" spans="1:20">
@@ -4604,7 +4604,7 @@
         <v>74</v>
       </c>
       <c r="T70">
-        <v>33</v>
+        <v>17.06896551724138</v>
       </c>
     </row>
     <row r="71" spans="1:20">
@@ -4725,7 +4725,7 @@
         <v>67.5</v>
       </c>
       <c r="T72">
-        <v>18</v>
+        <v>9.310344827586206</v>
       </c>
     </row>
     <row r="73" spans="1:20">
@@ -4843,7 +4843,7 @@
         <v>55</v>
       </c>
       <c r="T74">
-        <v>20</v>
+        <v>10.3448275862069</v>
       </c>
     </row>
     <row r="75" spans="1:20">
@@ -4905,7 +4905,7 @@
         <v>35</v>
       </c>
       <c r="T75">
-        <v>15</v>
+        <v>7.758620689655173</v>
       </c>
     </row>
     <row r="76" spans="1:20">

</xml_diff>

<commit_message>
Latest clean data verison
</commit_message>
<xml_diff>
--- a/data/clean/cleaned_data.xlsx
+++ b/data/clean/cleaned_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="27">
   <si>
     <t>Gesamtgruppe</t>
   </si>
@@ -79,7 +79,7 @@
     <t>Studierende</t>
   </si>
   <si>
-    <t>simulierte Daten</t>
+    <t>(simulierte Daten)</t>
   </si>
   <si>
     <t>männlich</t>
@@ -602,9 +602,6 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
       <c r="C3">
         <v>1</v>
       </c>
@@ -664,9 +661,6 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
       <c r="C4">
         <v>1</v>
       </c>
@@ -726,9 +720,6 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
       <c r="C5">
         <v>1</v>
       </c>
@@ -779,9 +770,6 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
       <c r="C6">
         <v>1</v>
       </c>
@@ -841,9 +829,6 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
       <c r="C7">
         <v>1</v>
       </c>
@@ -903,9 +888,6 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
       <c r="C8">
         <v>1</v>
       </c>
@@ -965,9 +947,6 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
       <c r="C9">
         <v>1</v>
       </c>
@@ -1027,9 +1006,6 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
       <c r="C10">
         <v>1</v>
       </c>
@@ -1056,9 +1032,6 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
       <c r="C11">
         <v>1</v>
       </c>
@@ -1118,9 +1091,6 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
       <c r="C12">
         <v>1</v>
       </c>
@@ -1180,9 +1150,6 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
       <c r="C13">
         <v>1</v>
       </c>
@@ -1242,9 +1209,6 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
       <c r="C14">
         <v>1</v>
       </c>
@@ -1295,9 +1259,6 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
       <c r="C15">
         <v>1</v>
       </c>
@@ -1357,9 +1318,6 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
       <c r="C16">
         <v>1</v>
       </c>
@@ -1416,9 +1374,6 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
       <c r="C17">
         <v>1</v>
       </c>
@@ -1469,9 +1424,6 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
       <c r="C18">
         <v>1</v>
       </c>
@@ -1528,9 +1480,6 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
       <c r="C19">
         <v>1</v>
       </c>
@@ -1587,9 +1536,6 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
       <c r="C20">
         <v>1</v>
       </c>
@@ -1649,9 +1595,6 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
       <c r="C21">
         <v>1</v>
       </c>
@@ -1711,9 +1654,6 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
       <c r="C22">
         <v>1</v>
       </c>
@@ -1773,9 +1713,6 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
       <c r="C23">
         <v>1</v>
       </c>
@@ -1820,9 +1757,6 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
       <c r="C24">
         <v>1</v>
       </c>
@@ -1878,9 +1812,6 @@
     <row r="25" spans="1:20">
       <c r="A25">
         <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>20</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1941,9 +1872,6 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>20</v>
-      </c>
       <c r="C26">
         <v>1</v>
       </c>
@@ -2003,9 +1931,6 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>20</v>
-      </c>
       <c r="C27">
         <v>1</v>
       </c>
@@ -2065,9 +1990,6 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
       <c r="C28">
         <v>1</v>
       </c>
@@ -2127,9 +2049,6 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>20</v>
-      </c>
       <c r="C29">
         <v>1</v>
       </c>
@@ -2186,9 +2105,6 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>20</v>
-      </c>
       <c r="C30">
         <v>1</v>
       </c>
@@ -2248,9 +2164,6 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>20</v>
-      </c>
       <c r="C31">
         <v>1</v>
       </c>
@@ -2307,9 +2220,6 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
-        <v>20</v>
-      </c>
       <c r="C32">
         <v>1</v>
       </c>
@@ -2369,9 +2279,6 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
-        <v>20</v>
-      </c>
       <c r="C33">
         <v>1</v>
       </c>
@@ -2428,9 +2335,6 @@
       <c r="A34">
         <v>34</v>
       </c>
-      <c r="B34" t="s">
-        <v>20</v>
-      </c>
       <c r="C34">
         <v>1</v>
       </c>
@@ -2487,9 +2391,6 @@
       <c r="A35">
         <v>35</v>
       </c>
-      <c r="B35" t="s">
-        <v>20</v>
-      </c>
       <c r="C35">
         <v>1</v>
       </c>
@@ -2546,9 +2447,6 @@
       <c r="A36">
         <v>36</v>
       </c>
-      <c r="B36" t="s">
-        <v>20</v>
-      </c>
       <c r="C36">
         <v>1</v>
       </c>
@@ -2605,9 +2503,6 @@
       <c r="A37">
         <v>37</v>
       </c>
-      <c r="B37" t="s">
-        <v>20</v>
-      </c>
       <c r="C37">
         <v>1</v>
       </c>
@@ -2664,9 +2559,6 @@
       <c r="A38">
         <v>38</v>
       </c>
-      <c r="B38" t="s">
-        <v>20</v>
-      </c>
       <c r="C38">
         <v>1</v>
       </c>
@@ -2726,9 +2618,6 @@
       <c r="A39">
         <v>39</v>
       </c>
-      <c r="B39" t="s">
-        <v>20</v>
-      </c>
       <c r="C39">
         <v>1</v>
       </c>
@@ -2782,9 +2671,6 @@
       <c r="A40">
         <v>40</v>
       </c>
-      <c r="B40" t="s">
-        <v>20</v>
-      </c>
       <c r="C40">
         <v>1</v>
       </c>
@@ -2841,9 +2727,6 @@
       <c r="A41">
         <v>41</v>
       </c>
-      <c r="B41" t="s">
-        <v>20</v>
-      </c>
       <c r="C41">
         <v>1</v>
       </c>
@@ -2903,9 +2786,6 @@
       <c r="A42">
         <v>42</v>
       </c>
-      <c r="B42" t="s">
-        <v>20</v>
-      </c>
       <c r="C42">
         <v>1</v>
       </c>
@@ -2965,9 +2845,6 @@
       <c r="A43">
         <v>43</v>
       </c>
-      <c r="B43" t="s">
-        <v>20</v>
-      </c>
       <c r="C43">
         <v>1</v>
       </c>
@@ -3024,9 +2901,6 @@
       <c r="A44">
         <v>44</v>
       </c>
-      <c r="B44" t="s">
-        <v>20</v>
-      </c>
       <c r="C44">
         <v>1</v>
       </c>
@@ -3074,9 +2948,6 @@
       <c r="A45">
         <v>45</v>
       </c>
-      <c r="B45" t="s">
-        <v>20</v>
-      </c>
       <c r="C45">
         <v>1</v>
       </c>
@@ -3136,9 +3007,6 @@
       <c r="A46">
         <v>46</v>
       </c>
-      <c r="B46" t="s">
-        <v>20</v>
-      </c>
       <c r="C46">
         <v>1</v>
       </c>
@@ -3186,9 +3054,6 @@
       <c r="A47">
         <v>47</v>
       </c>
-      <c r="B47" t="s">
-        <v>20</v>
-      </c>
       <c r="C47">
         <v>1</v>
       </c>
@@ -3236,9 +3101,6 @@
       <c r="A48">
         <v>48</v>
       </c>
-      <c r="B48" t="s">
-        <v>20</v>
-      </c>
       <c r="C48">
         <v>1</v>
       </c>
@@ -3298,9 +3160,6 @@
       <c r="A49">
         <v>49</v>
       </c>
-      <c r="B49" t="s">
-        <v>20</v>
-      </c>
       <c r="C49">
         <v>1</v>
       </c>
@@ -3360,9 +3219,6 @@
       <c r="A50">
         <v>50</v>
       </c>
-      <c r="B50" t="s">
-        <v>20</v>
-      </c>
       <c r="C50">
         <v>1</v>
       </c>
@@ -3413,9 +3269,6 @@
       <c r="A51">
         <v>51</v>
       </c>
-      <c r="B51" t="s">
-        <v>20</v>
-      </c>
       <c r="C51">
         <v>1</v>
       </c>
@@ -3472,9 +3325,6 @@
       <c r="A52">
         <v>52</v>
       </c>
-      <c r="B52" t="s">
-        <v>20</v>
-      </c>
       <c r="C52">
         <v>1</v>
       </c>
@@ -3531,9 +3381,6 @@
       <c r="A53">
         <v>53</v>
       </c>
-      <c r="B53" t="s">
-        <v>20</v>
-      </c>
       <c r="C53">
         <v>1</v>
       </c>
@@ -3584,9 +3431,6 @@
       <c r="A54">
         <v>54</v>
       </c>
-      <c r="B54" t="s">
-        <v>20</v>
-      </c>
       <c r="C54">
         <v>1</v>
       </c>
@@ -3646,9 +3490,6 @@
       <c r="A55">
         <v>55</v>
       </c>
-      <c r="B55" t="s">
-        <v>20</v>
-      </c>
       <c r="C55">
         <v>1</v>
       </c>
@@ -3708,9 +3549,6 @@
       <c r="A56">
         <v>56</v>
       </c>
-      <c r="B56" t="s">
-        <v>20</v>
-      </c>
       <c r="C56">
         <v>1</v>
       </c>
@@ -3770,9 +3608,6 @@
       <c r="A57">
         <v>57</v>
       </c>
-      <c r="B57" t="s">
-        <v>20</v>
-      </c>
       <c r="C57">
         <v>1</v>
       </c>
@@ -3826,9 +3661,6 @@
       <c r="A58">
         <v>58</v>
       </c>
-      <c r="B58" t="s">
-        <v>20</v>
-      </c>
       <c r="C58">
         <v>1</v>
       </c>
@@ -3888,9 +3720,6 @@
       <c r="A59">
         <v>59</v>
       </c>
-      <c r="B59" t="s">
-        <v>20</v>
-      </c>
       <c r="C59">
         <v>1</v>
       </c>
@@ -3950,9 +3779,6 @@
       <c r="A60">
         <v>60</v>
       </c>
-      <c r="B60" t="s">
-        <v>20</v>
-      </c>
       <c r="C60">
         <v>1</v>
       </c>
@@ -4009,9 +3835,6 @@
       <c r="A61">
         <v>61</v>
       </c>
-      <c r="B61" t="s">
-        <v>20</v>
-      </c>
       <c r="C61">
         <v>1</v>
       </c>
@@ -4071,9 +3894,6 @@
       <c r="A62">
         <v>62</v>
       </c>
-      <c r="B62" t="s">
-        <v>20</v>
-      </c>
       <c r="C62">
         <v>1</v>
       </c>
@@ -4133,9 +3953,6 @@
       <c r="A63">
         <v>63</v>
       </c>
-      <c r="B63" t="s">
-        <v>20</v>
-      </c>
       <c r="C63">
         <v>1</v>
       </c>
@@ -4189,9 +4006,6 @@
       <c r="A64">
         <v>64</v>
       </c>
-      <c r="B64" t="s">
-        <v>20</v>
-      </c>
       <c r="C64">
         <v>1</v>
       </c>
@@ -4251,12 +4065,6 @@
       <c r="A65">
         <v>65</v>
       </c>
-      <c r="B65" t="s">
-        <v>20</v>
-      </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
       <c r="D65" t="s">
         <v>23</v>
       </c>
@@ -4313,12 +4121,6 @@
       <c r="A66">
         <v>66</v>
       </c>
-      <c r="B66" t="s">
-        <v>20</v>
-      </c>
-      <c r="C66">
-        <v>1</v>
-      </c>
       <c r="D66" t="s">
         <v>23</v>
       </c>
@@ -4363,12 +4165,6 @@
       <c r="A67">
         <v>67</v>
       </c>
-      <c r="B67" t="s">
-        <v>20</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
       <c r="D67" t="s">
         <v>22</v>
       </c>
@@ -4425,12 +4221,6 @@
       <c r="A68">
         <v>68</v>
       </c>
-      <c r="B68" t="s">
-        <v>20</v>
-      </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
       <c r="D68" t="s">
         <v>23</v>
       </c>
@@ -4487,12 +4277,6 @@
       <c r="A69">
         <v>69</v>
       </c>
-      <c r="B69" t="s">
-        <v>20</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
       <c r="D69" t="s">
         <v>22</v>
       </c>
@@ -4549,12 +4333,6 @@
       <c r="A70">
         <v>70</v>
       </c>
-      <c r="B70" t="s">
-        <v>20</v>
-      </c>
-      <c r="C70">
-        <v>1</v>
-      </c>
       <c r="D70" t="s">
         <v>22</v>
       </c>
@@ -4611,12 +4389,6 @@
       <c r="A71">
         <v>71</v>
       </c>
-      <c r="B71" t="s">
-        <v>20</v>
-      </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
       <c r="D71" t="s">
         <v>22</v>
       </c>
@@ -4670,12 +4442,6 @@
       <c r="A72">
         <v>72</v>
       </c>
-      <c r="B72" t="s">
-        <v>20</v>
-      </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
       <c r="D72" t="s">
         <v>22</v>
       </c>
@@ -4732,12 +4498,6 @@
       <c r="A73">
         <v>73</v>
       </c>
-      <c r="B73" t="s">
-        <v>20</v>
-      </c>
-      <c r="C73">
-        <v>1</v>
-      </c>
       <c r="D73" t="s">
         <v>23</v>
       </c>
@@ -4788,12 +4548,6 @@
       <c r="A74">
         <v>74</v>
       </c>
-      <c r="B74" t="s">
-        <v>20</v>
-      </c>
-      <c r="C74">
-        <v>1</v>
-      </c>
       <c r="D74" t="s">
         <v>23</v>
       </c>
@@ -4850,12 +4604,6 @@
       <c r="A75">
         <v>75</v>
       </c>
-      <c r="B75" t="s">
-        <v>20</v>
-      </c>
-      <c r="C75">
-        <v>1</v>
-      </c>
       <c r="D75" t="s">
         <v>23</v>
       </c>
@@ -4944,9 +4692,6 @@
       <c r="A77">
         <v>2</v>
       </c>
-      <c r="B77" t="s">
-        <v>21</v>
-      </c>
       <c r="C77">
         <v>2</v>
       </c>
@@ -4976,9 +4721,6 @@
       <c r="A78">
         <v>3</v>
       </c>
-      <c r="B78" t="s">
-        <v>21</v>
-      </c>
       <c r="C78">
         <v>2</v>
       </c>
@@ -5008,9 +4750,6 @@
       <c r="A79">
         <v>4</v>
       </c>
-      <c r="B79" t="s">
-        <v>21</v>
-      </c>
       <c r="C79">
         <v>2</v>
       </c>
@@ -5040,9 +4779,6 @@
       <c r="A80">
         <v>5</v>
       </c>
-      <c r="B80" t="s">
-        <v>21</v>
-      </c>
       <c r="C80">
         <v>2</v>
       </c>
@@ -5072,9 +4808,6 @@
       <c r="A81">
         <v>6</v>
       </c>
-      <c r="B81" t="s">
-        <v>21</v>
-      </c>
       <c r="C81">
         <v>2</v>
       </c>
@@ -5104,9 +4837,6 @@
       <c r="A82">
         <v>7</v>
       </c>
-      <c r="B82" t="s">
-        <v>21</v>
-      </c>
       <c r="C82">
         <v>2</v>
       </c>
@@ -5136,9 +4866,6 @@
       <c r="A83">
         <v>8</v>
       </c>
-      <c r="B83" t="s">
-        <v>21</v>
-      </c>
       <c r="C83">
         <v>2</v>
       </c>
@@ -5168,9 +4895,6 @@
       <c r="A84">
         <v>9</v>
       </c>
-      <c r="B84" t="s">
-        <v>21</v>
-      </c>
       <c r="C84">
         <v>2</v>
       </c>
@@ -5200,9 +4924,6 @@
       <c r="A85">
         <v>10</v>
       </c>
-      <c r="B85" t="s">
-        <v>21</v>
-      </c>
       <c r="C85">
         <v>2</v>
       </c>
@@ -5232,9 +4953,6 @@
       <c r="A86">
         <v>11</v>
       </c>
-      <c r="B86" t="s">
-        <v>21</v>
-      </c>
       <c r="C86">
         <v>2</v>
       </c>
@@ -5264,9 +4982,6 @@
       <c r="A87">
         <v>12</v>
       </c>
-      <c r="B87" t="s">
-        <v>21</v>
-      </c>
       <c r="C87">
         <v>2</v>
       </c>
@@ -5296,9 +5011,6 @@
       <c r="A88">
         <v>14</v>
       </c>
-      <c r="B88" t="s">
-        <v>21</v>
-      </c>
       <c r="C88">
         <v>2</v>
       </c>
@@ -5328,9 +5040,6 @@
       <c r="A89">
         <v>15</v>
       </c>
-      <c r="B89" t="s">
-        <v>21</v>
-      </c>
       <c r="C89">
         <v>2</v>
       </c>
@@ -5360,9 +5069,6 @@
       <c r="A90">
         <v>17</v>
       </c>
-      <c r="B90" t="s">
-        <v>21</v>
-      </c>
       <c r="C90">
         <v>2</v>
       </c>
@@ -5392,9 +5098,6 @@
       <c r="A91">
         <v>18</v>
       </c>
-      <c r="B91" t="s">
-        <v>21</v>
-      </c>
       <c r="C91">
         <v>2</v>
       </c>
@@ -5424,9 +5127,6 @@
       <c r="A92">
         <v>19</v>
       </c>
-      <c r="B92" t="s">
-        <v>21</v>
-      </c>
       <c r="C92">
         <v>2</v>
       </c>
@@ -5456,9 +5156,6 @@
       <c r="A93">
         <v>20</v>
       </c>
-      <c r="B93" t="s">
-        <v>21</v>
-      </c>
       <c r="C93">
         <v>2</v>
       </c>
@@ -5488,9 +5185,6 @@
       <c r="A94">
         <v>21</v>
       </c>
-      <c r="B94" t="s">
-        <v>21</v>
-      </c>
       <c r="C94">
         <v>2</v>
       </c>
@@ -5520,9 +5214,6 @@
       <c r="A95">
         <v>22</v>
       </c>
-      <c r="B95" t="s">
-        <v>21</v>
-      </c>
       <c r="C95">
         <v>2</v>
       </c>
@@ -5552,9 +5243,6 @@
       <c r="A96">
         <v>23</v>
       </c>
-      <c r="B96" t="s">
-        <v>21</v>
-      </c>
       <c r="C96">
         <v>2</v>
       </c>
@@ -5583,9 +5271,6 @@
     <row r="97" spans="1:10">
       <c r="A97">
         <v>24</v>
-      </c>
-      <c r="B97" t="s">
-        <v>21</v>
       </c>
       <c r="C97">
         <v>2</v>
@@ -5615,9 +5300,6 @@
     <row r="98" spans="1:10">
       <c r="A98">
         <v>25</v>
-      </c>
-      <c r="B98" t="s">
-        <v>21</v>
       </c>
       <c r="C98">
         <v>2</v>

</xml_diff>